<commit_message>
UI now correctly displays responses from bot
</commit_message>
<xml_diff>
--- a/PROS_timesheet.xlsx
+++ b/PROS_timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andres\Documents\Personal\Coding Challenges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F170E1-1577-4A97-AD0A-089844F35FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDE90E9-E4D1-4309-95B5-A000DADC7B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8EFE6B73-BA09-4E99-B916-0C8EF1FF0D30}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
   <si>
     <t>Time</t>
   </si>
@@ -114,6 +114,36 @@
   </si>
   <si>
     <t>https://github.com/MacksEntropy/Codered_PROS/commit/59bf34f1f345a029cbf6076eb67ed07c3a1ebb1d</t>
+  </si>
+  <si>
+    <t>Set up API for chatbot</t>
+  </si>
+  <si>
+    <t>https://github.com/MacksEntropy/Codered_PROS/commit/9cb76374efcfad71c65d0a7f6a3ed6410bbdb092</t>
+  </si>
+  <si>
+    <t>Created initial webapp</t>
+  </si>
+  <si>
+    <t>https://github.com/MacksEntropy/Codered_PROS/commit/010064c5cbbd2c7238423fb262a4eac12a7b0ec1</t>
+  </si>
+  <si>
+    <t>Fixed bug with user messages</t>
+  </si>
+  <si>
+    <t>https://github.com/MacksEntropy/Codered_PROS/commit/acf64b97b66b5924c38c1b902585c72d6ff6c134</t>
+  </si>
+  <si>
+    <t>https://github.com/MacksEntropy/Codered_PROS/commit/3537c190539025050d1bff98e59dd164c23b17d1</t>
+  </si>
+  <si>
+    <t>https://github.com/MacksEntropy/Codered_PROS/commit/a35d5a790100420e49193f5c4f9f70a46d787f4c</t>
+  </si>
+  <si>
+    <t>Refactored nlp module for conversation like dialouge</t>
+  </si>
+  <si>
+    <t>Created framework for backend API</t>
   </si>
 </sst>
 </file>
@@ -484,13 +514,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6528202E-6A02-44D7-B252-69B48F3BC957}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21:I22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="45" customWidth="1"/>
     <col min="3" max="3" width="11.109375" customWidth="1"/>
     <col min="4" max="4" width="98.109375" customWidth="1"/>
   </cols>
@@ -760,45 +790,114 @@
       <c r="A22">
         <v>10.5</v>
       </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>11</v>
       </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>11.5</v>
       </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>12</v>
       </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>12.5</v>
       </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>13</v>
       </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>13.5</v>
       </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>14</v>
       </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>14.5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>